<commit_message>
new data, new org, all millimolar!!
</commit_message>
<xml_diff>
--- a/data/LCMS_Standards.xlsx
+++ b/data/LCMS_Standards.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\ECFERS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7969D8DD-2F9C-40EE-9A9A-B5CD0FD9948D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BD1AC6-E154-415A-B53E-914F2B1F928A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17835" yWindow="1380" windowWidth="14685" windowHeight="16725" xr2:uid="{A5058EDE-1C8B-C345-BCDB-7FCA08701FCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A5058EDE-1C8B-C345-BCDB-7FCA08701FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Metabolite</t>
   </si>
@@ -44,27 +44,9 @@
     <t>Equation</t>
   </si>
   <si>
-    <t>Malate</t>
-  </si>
-  <si>
-    <t>Y = 6370907*X + 428300</t>
-  </si>
-  <si>
-    <t>Pyruvate</t>
-  </si>
-  <si>
-    <t>Y = 673731*X - 18732</t>
-  </si>
-  <si>
-    <t>Serine</t>
-  </si>
-  <si>
     <t>Y = 1943043*X + 44972</t>
   </si>
   <si>
-    <t>Glycine</t>
-  </si>
-  <si>
     <t>Y = 105851*X + 1257</t>
   </si>
   <si>
@@ -83,18 +65,12 @@
     <t>5,10-CH=THF</t>
   </si>
   <si>
-    <t>Y = 86009*X + 624.0</t>
-  </si>
-  <si>
     <t>5,10-CH2-THF</t>
   </si>
   <si>
     <t>Y = 2230633*X - 82838</t>
   </si>
   <si>
-    <t>Y = 726472*X - 52.49</t>
-  </si>
-  <si>
     <t>NADP</t>
   </si>
   <si>
@@ -107,21 +83,12 @@
     <t>NADH</t>
   </si>
   <si>
-    <t>Y = 1317228*X + 16723</t>
-  </si>
-  <si>
     <t>NAD</t>
   </si>
   <si>
     <t>Y = 1437245*X + 19317</t>
   </si>
   <si>
-    <t>CoA</t>
-  </si>
-  <si>
-    <t>acetyl-CoA</t>
-  </si>
-  <si>
     <t>Y = 4228479*X - 185859</t>
   </si>
   <si>
@@ -131,32 +98,113 @@
     <t>Y = 7610507*X + 211001</t>
   </si>
   <si>
-    <t>Y = 3116110*X + 180994</t>
-  </si>
-  <si>
-    <t>Succinate</t>
-  </si>
-  <si>
     <t>Y = 2484862*X + 142079</t>
   </si>
   <si>
-    <t>Fumarate</t>
-  </si>
-  <si>
-    <t>Y = 5931770*X + 4598311</t>
-  </si>
-  <si>
-    <t>Citrate</t>
-  </si>
-  <si>
-    <t>Y = 78356408*X + 10610249</t>
+    <t>acetylcoa</t>
+  </si>
+  <si>
+    <t>malate</t>
+  </si>
+  <si>
+    <t>pyruvate</t>
+  </si>
+  <si>
+    <t>serine</t>
+  </si>
+  <si>
+    <t>glycine</t>
+  </si>
+  <si>
+    <t>coa</t>
+  </si>
+  <si>
+    <t>succinate</t>
+  </si>
+  <si>
+    <t>fumarate</t>
+  </si>
+  <si>
+    <t>citrate</t>
+  </si>
+  <si>
+    <t>atp</t>
+  </si>
+  <si>
+    <t>malonylcoa</t>
+  </si>
+  <si>
+    <t>Y = 624609*X - 78120</t>
+  </si>
+  <si>
+    <t>glyoxylate</t>
+  </si>
+  <si>
+    <t>Y = 1772799*X - 105149</t>
+  </si>
+  <si>
+    <t>alanine</t>
+  </si>
+  <si>
+    <t>aspartate</t>
+  </si>
+  <si>
+    <t>lysine</t>
+  </si>
+  <si>
+    <t>valine</t>
+  </si>
+  <si>
+    <t>hydroxyglutarate</t>
+  </si>
+  <si>
+    <t>oxobutanoate</t>
+  </si>
+  <si>
+    <t>Y = 32648315*X - 77085</t>
+  </si>
+  <si>
+    <t>Y = 4208000*X + 430070</t>
+  </si>
+  <si>
+    <t>Y = 1305521*X + 219238</t>
+  </si>
+  <si>
+    <t>Y = 86009*X + 624</t>
+  </si>
+  <si>
+    <t>Y = 726472*X - 52</t>
+  </si>
+  <si>
+    <t>Y = 5118279*X + 77819</t>
+  </si>
+  <si>
+    <t>Y = 2594733*X + 8677</t>
+  </si>
+  <si>
+    <t>Y = 4320042*X + 211833</t>
+  </si>
+  <si>
+    <t>Y = 5148733*X + 385969</t>
+  </si>
+  <si>
+    <t>Y = 7612645*X - 466166</t>
+  </si>
+  <si>
+    <t>Y = 3715504*X + 169087</t>
+  </si>
+  <si>
+    <t>Y = 4426423*X + 7569</t>
+  </si>
+  <si>
+    <t>Y = 123565436*X + 2698669</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,6 +238,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,12 +265,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,15 +588,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A264EAB0-40B5-684B-85A7-72AAACD51255}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,156 +607,217 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>230511</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2">
-        <v>230131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12">
-        <v>230630</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>